<commit_message>
pushed from the office system
</commit_message>
<xml_diff>
--- a/Configuration/Experts-Staging-TestData-ExcelSheet.xlsx
+++ b/Configuration/Experts-Staging-TestData-ExcelSheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Password</t>
   </si>
@@ -52,12 +52,6 @@
   </si>
   <si>
     <t xml:space="preserve">Mobile Number </t>
-  </si>
-  <si>
-    <t>cvvcbvn</t>
-  </si>
-  <si>
-    <t>hgjhgjhgj</t>
   </si>
 </sst>
 </file>
@@ -419,7 +413,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,8 +455,8 @@
       <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
+      <c r="E2">
+        <v>1234567890</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -478,8 +472,8 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
+      <c r="E3">
+        <v>2112345678</v>
       </c>
     </row>
   </sheetData>

</xml_diff>